<commit_message>
IMG updates + lvl updates
</commit_message>
<xml_diff>
--- a/data/Level_Robbe.xlsx
+++ b/data/Level_Robbe.xlsx
@@ -372,8 +372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:KN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CW1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="DE4" sqref="DE4"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BB6" sqref="BB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -536,13 +536,13 @@
         <v>0</v>
       </c>
       <c r="BA1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BC1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD1">
         <v>3</v>
@@ -686,16 +686,16 @@
         <v>0</v>
       </c>
       <c r="CY1">
+        <v>0</v>
+      </c>
+      <c r="CZ1">
+        <v>0</v>
+      </c>
+      <c r="DA1">
+        <v>0</v>
+      </c>
+      <c r="DB1">
         <v>6</v>
-      </c>
-      <c r="CZ1">
-        <v>0</v>
-      </c>
-      <c r="DA1">
-        <v>0</v>
-      </c>
-      <c r="DB1">
-        <v>0</v>
       </c>
       <c r="DC1">
         <v>0</v>
@@ -1438,13 +1438,13 @@
         <v>0</v>
       </c>
       <c r="BA2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BC2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BD2">
         <v>8</v>
@@ -1588,7 +1588,7 @@
         <v>0</v>
       </c>
       <c r="CY2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="CZ2">
         <v>0</v>
@@ -1597,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="DB2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DC2">
         <v>0</v>
@@ -1609,25 +1609,25 @@
         <v>0</v>
       </c>
       <c r="DF2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="DG2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="DH2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="DI2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="DJ2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DK2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DL2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DM2">
         <v>0</v>
@@ -2340,7 +2340,7 @@
         <v>0</v>
       </c>
       <c r="BA3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BB3">
         <v>0</v>
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="BD3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BE3">
         <v>0</v>
@@ -5043,10 +5043,10 @@
         <v>0</v>
       </c>
       <c r="AZ6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BB6">
         <v>0</v>
@@ -5945,7 +5945,7 @@
         <v>0</v>
       </c>
       <c r="AZ7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA7">
         <v>3</v>
@@ -7018,10 +7018,10 @@
         <v>0</v>
       </c>
       <c r="DE8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="DF8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DG8">
         <v>8</v>
@@ -7036,10 +7036,10 @@
         <v>8</v>
       </c>
       <c r="DK8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="DL8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="DM8">
         <v>0</v>
@@ -7944,25 +7944,25 @@
         <v>1</v>
       </c>
       <c r="DM9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DN9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DO9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DP9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DQ9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DR9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DS9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DT9">
         <v>0</v>

</xml_diff>

<commit_message>
update voor spikes in alle richtingen
</commit_message>
<xml_diff>
--- a/data/Level_Robbe.xlsx
+++ b/data/Level_Robbe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17253" windowHeight="5667"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5670"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -370,15 +370,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:KN9"/>
+  <dimension ref="A1:KO9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BB6" sqref="BB6"/>
+    <sheetView tabSelected="1" topLeftCell="DB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="DQ8" sqref="DQ8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:300" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:301" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>3</v>
       </c>
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="BA1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BB1">
         <v>3</v>
@@ -548,7 +548,7 @@
         <v>3</v>
       </c>
       <c r="BE1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF1">
         <v>0</v>
@@ -653,14 +653,14 @@
         <v>0</v>
       </c>
       <c r="CN1">
+        <v>0</v>
+      </c>
+      <c r="CO1">
         <v>8</v>
       </c>
-      <c r="CO1">
+      <c r="CP1">
         <v>3</v>
       </c>
-      <c r="CP1">
-        <v>0</v>
-      </c>
       <c r="CQ1">
         <v>0</v>
       </c>
@@ -695,14 +695,14 @@
         <v>0</v>
       </c>
       <c r="DB1">
+        <v>0</v>
+      </c>
+      <c r="DC1">
+        <v>0</v>
+      </c>
+      <c r="DD1">
         <v>6</v>
       </c>
-      <c r="DC1">
-        <v>0</v>
-      </c>
-      <c r="DD1">
-        <v>0</v>
-      </c>
       <c r="DE1">
         <v>0</v>
       </c>
@@ -752,10 +752,10 @@
         <v>0</v>
       </c>
       <c r="DU1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="DV1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="DW1">
         <v>0</v>
@@ -1277,10 +1277,13 @@
         <v>0</v>
       </c>
       <c r="KN1">
+        <v>0</v>
+      </c>
+      <c r="KO1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:300" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:301" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1438,10 +1441,10 @@
         <v>0</v>
       </c>
       <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
         <v>3</v>
-      </c>
-      <c r="BB2">
-        <v>8</v>
       </c>
       <c r="BC2">
         <v>8</v>
@@ -1450,7 +1453,7 @@
         <v>8</v>
       </c>
       <c r="BE2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BF2">
         <v>0</v>
@@ -1555,14 +1558,14 @@
         <v>0</v>
       </c>
       <c r="CN2">
+        <v>0</v>
+      </c>
+      <c r="CO2">
         <v>8</v>
       </c>
-      <c r="CO2">
+      <c r="CP2">
         <v>3</v>
       </c>
-      <c r="CP2">
-        <v>0</v>
-      </c>
       <c r="CQ2">
         <v>0</v>
       </c>
@@ -1597,37 +1600,37 @@
         <v>0</v>
       </c>
       <c r="DB2">
+        <v>0</v>
+      </c>
+      <c r="DC2">
+        <v>0</v>
+      </c>
+      <c r="DD2">
         <v>4</v>
       </c>
-      <c r="DC2">
-        <v>0</v>
-      </c>
-      <c r="DD2">
-        <v>0</v>
-      </c>
       <c r="DE2">
         <v>0</v>
       </c>
       <c r="DF2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DG2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DH2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DI2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DJ2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DK2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DL2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DM2">
         <v>0</v>
@@ -2179,10 +2182,13 @@
         <v>0</v>
       </c>
       <c r="KN2">
+        <v>0</v>
+      </c>
+      <c r="KO2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:300" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:301" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2340,11 +2346,11 @@
         <v>0</v>
       </c>
       <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
         <v>8</v>
       </c>
-      <c r="BB3">
-        <v>0</v>
-      </c>
       <c r="BC3">
         <v>0</v>
       </c>
@@ -2457,14 +2463,14 @@
         <v>0</v>
       </c>
       <c r="CN3">
+        <v>0</v>
+      </c>
+      <c r="CO3">
         <v>8</v>
       </c>
-      <c r="CO3">
+      <c r="CP3">
         <v>3</v>
       </c>
-      <c r="CP3">
-        <v>0</v>
-      </c>
       <c r="CQ3">
         <v>0</v>
       </c>
@@ -2514,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="DG3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="DH3">
         <v>0</v>
@@ -2526,25 +2532,25 @@
         <v>0</v>
       </c>
       <c r="DK3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DL3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DM3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DN3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DO3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DP3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DQ3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DR3">
         <v>0</v>
@@ -3081,10 +3087,13 @@
         <v>0</v>
       </c>
       <c r="KN3">
+        <v>0</v>
+      </c>
+      <c r="KO3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:300" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:301" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3173,11 +3182,11 @@
         <v>0</v>
       </c>
       <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
         <v>3</v>
       </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
       <c r="AF4">
         <v>0</v>
       </c>
@@ -3272,7 +3281,7 @@
         <v>0</v>
       </c>
       <c r="BK4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BL4">
         <v>3</v>
@@ -3341,7 +3350,7 @@
         <v>3</v>
       </c>
       <c r="CH4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CI4">
         <v>0</v>
@@ -3359,14 +3368,14 @@
         <v>0</v>
       </c>
       <c r="CN4">
+        <v>0</v>
+      </c>
+      <c r="CO4">
         <v>8</v>
       </c>
-      <c r="CO4">
+      <c r="CP4">
         <v>3</v>
       </c>
-      <c r="CP4">
-        <v>0</v>
-      </c>
       <c r="CQ4">
         <v>0</v>
       </c>
@@ -3425,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="DJ4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DK4">
         <v>0</v>
@@ -3983,10 +3992,13 @@
         <v>0</v>
       </c>
       <c r="KN4">
+        <v>0</v>
+      </c>
+      <c r="KO4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:300" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:301" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4066,11 +4078,11 @@
         <v>0</v>
       </c>
       <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
         <v>3</v>
       </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
       <c r="AC5">
         <v>0</v>
       </c>
@@ -4189,11 +4201,11 @@
         <v>0</v>
       </c>
       <c r="BP5">
+        <v>0</v>
+      </c>
+      <c r="BQ5">
         <v>8</v>
       </c>
-      <c r="BQ5">
-        <v>0</v>
-      </c>
       <c r="BR5">
         <v>0</v>
       </c>
@@ -4207,11 +4219,11 @@
         <v>0</v>
       </c>
       <c r="BV5">
+        <v>0</v>
+      </c>
+      <c r="BW5">
         <v>8</v>
       </c>
-      <c r="BW5">
-        <v>0</v>
-      </c>
       <c r="BX5">
         <v>0</v>
       </c>
@@ -4225,14 +4237,14 @@
         <v>0</v>
       </c>
       <c r="CB5">
+        <v>0</v>
+      </c>
+      <c r="CC5">
         <v>8</v>
       </c>
-      <c r="CC5">
+      <c r="CD5">
         <v>3</v>
       </c>
-      <c r="CD5">
-        <v>0</v>
-      </c>
       <c r="CE5">
         <v>0</v>
       </c>
@@ -4261,14 +4273,14 @@
         <v>0</v>
       </c>
       <c r="CN5">
+        <v>0</v>
+      </c>
+      <c r="CO5">
         <v>8</v>
       </c>
-      <c r="CO5">
+      <c r="CP5">
         <v>3</v>
       </c>
-      <c r="CP5">
-        <v>0</v>
-      </c>
       <c r="CQ5">
         <v>0</v>
       </c>
@@ -4324,10 +4336,10 @@
         <v>0</v>
       </c>
       <c r="DI5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DJ5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="DK5">
         <v>0</v>
@@ -4885,10 +4897,13 @@
         <v>0</v>
       </c>
       <c r="KN5">
+        <v>0</v>
+      </c>
+      <c r="KO5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:300" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:301" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4959,11 +4974,11 @@
         <v>0</v>
       </c>
       <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
         <v>3</v>
       </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
       <c r="Z6">
         <v>0</v>
       </c>
@@ -5043,11 +5058,11 @@
         <v>0</v>
       </c>
       <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BA6">
         <v>3</v>
       </c>
-      <c r="BA6">
-        <v>0</v>
-      </c>
       <c r="BB6">
         <v>0</v>
       </c>
@@ -5055,11 +5070,11 @@
         <v>0</v>
       </c>
       <c r="BD6">
+        <v>0</v>
+      </c>
+      <c r="BE6">
         <v>8</v>
       </c>
-      <c r="BE6">
-        <v>0</v>
-      </c>
       <c r="BF6">
         <v>0</v>
       </c>
@@ -5130,11 +5145,11 @@
         <v>0</v>
       </c>
       <c r="CC6">
+        <v>0</v>
+      </c>
+      <c r="CD6">
         <v>8</v>
       </c>
-      <c r="CD6">
-        <v>0</v>
-      </c>
       <c r="CE6">
         <v>0</v>
       </c>
@@ -5163,14 +5178,14 @@
         <v>0</v>
       </c>
       <c r="CN6">
+        <v>0</v>
+      </c>
+      <c r="CO6">
         <v>8</v>
       </c>
-      <c r="CO6">
+      <c r="CP6">
         <v>3</v>
       </c>
-      <c r="CP6">
-        <v>0</v>
-      </c>
       <c r="CQ6">
         <v>0</v>
       </c>
@@ -5223,13 +5238,13 @@
         <v>0</v>
       </c>
       <c r="DH6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DI6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="DJ6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="DK6">
         <v>0</v>
@@ -5787,10 +5802,13 @@
         <v>0</v>
       </c>
       <c r="KN6">
+        <v>0</v>
+      </c>
+      <c r="KO6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:300" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:301" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -5852,11 +5870,11 @@
         <v>0</v>
       </c>
       <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>3</v>
       </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
       <c r="W7">
         <v>0</v>
       </c>
@@ -5939,13 +5957,13 @@
         <v>0</v>
       </c>
       <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
         <v>3</v>
       </c>
-      <c r="AY7">
-        <v>0</v>
-      </c>
       <c r="AZ7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BA7">
         <v>3</v>
@@ -5960,7 +5978,7 @@
         <v>3</v>
       </c>
       <c r="BE7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF7">
         <v>0</v>
@@ -5984,11 +6002,11 @@
         <v>0</v>
       </c>
       <c r="BM7">
+        <v>0</v>
+      </c>
+      <c r="BN7">
         <v>8</v>
       </c>
-      <c r="BN7">
-        <v>0</v>
-      </c>
       <c r="BO7">
         <v>0</v>
       </c>
@@ -6002,11 +6020,11 @@
         <v>0</v>
       </c>
       <c r="BS7">
+        <v>0</v>
+      </c>
+      <c r="BT7">
         <v>8</v>
       </c>
-      <c r="BT7">
-        <v>0</v>
-      </c>
       <c r="BU7">
         <v>0</v>
       </c>
@@ -6020,11 +6038,11 @@
         <v>0</v>
       </c>
       <c r="BY7">
+        <v>0</v>
+      </c>
+      <c r="BZ7">
         <v>8</v>
       </c>
-      <c r="BZ7">
-        <v>0</v>
-      </c>
       <c r="CA7">
         <v>0</v>
       </c>
@@ -6044,11 +6062,11 @@
         <v>0</v>
       </c>
       <c r="CG7">
+        <v>0</v>
+      </c>
+      <c r="CH7">
         <v>8</v>
       </c>
-      <c r="CH7">
-        <v>0</v>
-      </c>
       <c r="CI7">
         <v>0</v>
       </c>
@@ -6065,14 +6083,14 @@
         <v>0</v>
       </c>
       <c r="CN7">
+        <v>0</v>
+      </c>
+      <c r="CO7">
         <v>8</v>
       </c>
-      <c r="CO7">
+      <c r="CP7">
         <v>3</v>
       </c>
-      <c r="CP7">
-        <v>0</v>
-      </c>
       <c r="CQ7">
         <v>0</v>
       </c>
@@ -6116,7 +6134,7 @@
         <v>0</v>
       </c>
       <c r="DE7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DF7">
         <v>0</v>
@@ -6689,10 +6707,13 @@
         <v>0</v>
       </c>
       <c r="KN7">
+        <v>0</v>
+      </c>
+      <c r="KO7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:300" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:301" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -6745,11 +6766,11 @@
         <v>0</v>
       </c>
       <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
         <v>3</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
       <c r="T8">
         <v>0</v>
       </c>
@@ -6784,7 +6805,7 @@
         <v>0</v>
       </c>
       <c r="AE8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AF8">
         <v>8</v>
@@ -6793,7 +6814,7 @@
         <v>8</v>
       </c>
       <c r="AH8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -6802,11 +6823,11 @@
         <v>0</v>
       </c>
       <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
         <v>8</v>
       </c>
-      <c r="AL8">
-        <v>0</v>
-      </c>
       <c r="AM8">
         <v>0</v>
       </c>
@@ -6814,11 +6835,11 @@
         <v>0</v>
       </c>
       <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
         <v>8</v>
       </c>
-      <c r="AP8">
-        <v>0</v>
-      </c>
       <c r="AQ8">
         <v>0</v>
       </c>
@@ -6832,11 +6853,11 @@
         <v>0</v>
       </c>
       <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
         <v>3</v>
       </c>
-      <c r="AV8">
-        <v>0</v>
-      </c>
       <c r="AW8">
         <v>0</v>
       </c>
@@ -6880,7 +6901,7 @@
         <v>0</v>
       </c>
       <c r="BK8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BL8">
         <v>3</v>
@@ -6949,17 +6970,17 @@
         <v>3</v>
       </c>
       <c r="CH8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CI8">
         <v>0</v>
       </c>
       <c r="CJ8">
+        <v>0</v>
+      </c>
+      <c r="CK8">
         <v>8</v>
       </c>
-      <c r="CK8">
-        <v>0</v>
-      </c>
       <c r="CL8">
         <v>0</v>
       </c>
@@ -6982,35 +7003,35 @@
         <v>0</v>
       </c>
       <c r="CS8">
+        <v>0</v>
+      </c>
+      <c r="CT8">
         <v>10</v>
       </c>
-      <c r="CT8">
-        <v>0</v>
-      </c>
       <c r="CU8">
         <v>0</v>
       </c>
       <c r="CV8">
+        <v>0</v>
+      </c>
+      <c r="CW8">
         <v>10</v>
       </c>
-      <c r="CW8">
-        <v>0</v>
-      </c>
       <c r="CX8">
+        <v>0</v>
+      </c>
+      <c r="CY8">
         <v>10</v>
       </c>
-      <c r="CY8">
-        <v>0</v>
-      </c>
       <c r="CZ8">
         <v>0</v>
       </c>
       <c r="DA8">
+        <v>0</v>
+      </c>
+      <c r="DB8">
         <v>10</v>
       </c>
-      <c r="DB8">
-        <v>0</v>
-      </c>
       <c r="DC8">
         <v>0</v>
       </c>
@@ -7018,10 +7039,10 @@
         <v>0</v>
       </c>
       <c r="DE8">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="DF8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="DG8">
         <v>8</v>
@@ -7042,10 +7063,10 @@
         <v>8</v>
       </c>
       <c r="DM8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="DN8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="DO8">
         <v>0</v>
@@ -7075,7 +7096,7 @@
         <v>0</v>
       </c>
       <c r="DX8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="DY8">
         <v>0</v>
@@ -7591,10 +7612,13 @@
         <v>0</v>
       </c>
       <c r="KN8">
+        <v>0</v>
+      </c>
+      <c r="KO8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:300" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:301" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -7686,7 +7710,7 @@
         <v>0</v>
       </c>
       <c r="AE9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF9">
         <v>1</v>
@@ -7728,7 +7752,7 @@
         <v>1</v>
       </c>
       <c r="AS9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT9">
         <v>2</v>
@@ -7764,7 +7788,7 @@
         <v>2</v>
       </c>
       <c r="BE9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BF9">
         <v>1</v>
@@ -7782,7 +7806,7 @@
         <v>1</v>
       </c>
       <c r="BK9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BL9">
         <v>2</v>
@@ -7848,7 +7872,7 @@
         <v>2</v>
       </c>
       <c r="CG9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CH9">
         <v>1</v>
@@ -7881,7 +7905,7 @@
         <v>1</v>
       </c>
       <c r="CR9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CS9">
         <v>2</v>
@@ -7911,7 +7935,7 @@
         <v>2</v>
       </c>
       <c r="DB9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DC9">
         <v>1</v>
@@ -7965,40 +7989,40 @@
         <v>1</v>
       </c>
       <c r="DT9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DU9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DV9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DW9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DX9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DY9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DZ9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EA9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EB9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EC9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ED9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EE9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EF9">
         <v>0</v>
@@ -8493,6 +8517,9 @@
         <v>0</v>
       </c>
       <c r="KN9">
+        <v>0</v>
+      </c>
+      <c r="KO9">
         <v>0</v>
       </c>
     </row>

</xml_diff>